<commit_message>
add calculo de média e balanceamento de classe
</commit_message>
<xml_diff>
--- a/src/data/result_mean.xlsx
+++ b/src/data/result_mean.xlsx
@@ -497,22 +497,22 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.914588235294118</v>
+        <v>3.897971727105102</v>
       </c>
       <c r="B3" t="n">
-        <v>2.273764705882353</v>
+        <v>2.263060848186847</v>
       </c>
       <c r="C3" t="n">
-        <v>2.356352941176471</v>
+        <v>2.338660110633067</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7725095294117648</v>
+        <v>0.7713847572218808</v>
       </c>
       <c r="E3" t="n">
-        <v>68.67258823529411</v>
+        <v>68.44253226797787</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2964117647058824</v>
+        <v>0.2904585125998771</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>

</xml_diff>